<commit_message>
Semana 3 | dia 1 | Desarrollo de Datamart OEC
</commit_message>
<xml_diff>
--- a/2_data_understanding_module/collecting_initial_data/additional_data/costos_de_cursos_cec_epn.xlsx
+++ b/2_data_understanding_module/collecting_initial_data/additional_data/costos_de_cursos_cec_epn.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\University\TESIS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\University\Data-Mining-System-SETEC\2_data_understanding_module\collecting_initial_data\additional_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B1D43A-5321-46CB-A15B-4635AC211897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3240A601-5D24-4287-92E3-A5713BB8EAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D9F23ADD-436A-400B-A967-49B7C46C677B}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>Área</t>
   </si>
   <si>
-    <t>Business Intelligence</t>
-  </si>
-  <si>
     <t>Power BI 2: Funciones QUERY y DAX</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
     <t>Python Essentials</t>
   </si>
   <si>
-    <t>Desarrollo de Software</t>
-  </si>
-  <si>
     <t>Excel</t>
   </si>
   <si>
@@ -119,9 +113,6 @@
     <t>Machine Learning con R</t>
   </si>
   <si>
-    <t>Programación</t>
-  </si>
-  <si>
     <t>Project</t>
   </si>
   <si>
@@ -129,6 +120,15 @@
   </si>
   <si>
     <t>Microsoft Project Avanzado</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>Programación en R</t>
   </si>
 </sst>
 </file>
@@ -485,14 +485,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40BE872A-E7F0-40C7-9B0E-6F8F285D4164}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21" style="1" customWidth="1"/>
+    <col min="2" max="2" width="77.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5546875" style="1" customWidth="1"/>
@@ -517,13 +517,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1">
         <v>24</v>
@@ -532,15 +532,15 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1">
         <v>24</v>
@@ -549,15 +549,15 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1">
         <v>24</v>
@@ -568,47 +568,47 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E5" s="1">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="1">
-        <v>24</v>
-      </c>
-      <c r="E6" s="1">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1">
         <v>32</v>
@@ -617,15 +617,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1">
         <v>32</v>
@@ -634,15 +634,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D9" s="1">
         <v>24</v>
@@ -651,15 +651,15 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="1">
         <v>48</v>
@@ -668,15 +668,15 @@
         <v>140</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="1">
         <v>48</v>
@@ -685,15 +685,15 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="1">
         <v>24</v>
@@ -702,15 +702,15 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="1">
         <v>24</v>
@@ -719,15 +719,15 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14" s="1">
         <v>24</v>
@@ -736,15 +736,15 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D15" s="1">
         <v>24</v>
@@ -753,15 +753,15 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D16" s="1">
         <v>24</v>
@@ -770,15 +770,15 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D17" s="1">
         <v>24</v>
@@ -787,15 +787,15 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="C18" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D18" s="1">
         <v>120</v>
@@ -804,15 +804,15 @@
         <v>540</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19" s="1">
         <v>32</v>
@@ -823,13 +823,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D20" s="1">
         <v>40</v>
@@ -838,15 +838,15 @@
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D21" s="1">
         <v>140</v>
@@ -857,13 +857,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D22" s="1">
         <v>140</v>

</xml_diff>

<commit_message>
Semana 14| Dia 2| Desarrollo del documento y reestructuracion de archivos del proyecto
</commit_message>
<xml_diff>
--- a/2_data_understanding_module/collecting_initial_data/additional_data/costos_de_cursos_cec_epn.xlsx
+++ b/2_data_understanding_module/collecting_initial_data/additional_data/costos_de_cursos_cec_epn.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\University\Data-Mining-System-SETEC\2_data_understanding_module\collecting_initial_data\additional_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CFF02F-FE26-45CD-9F23-BFA6A55D3422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA3AE36-0A7C-44E2-95FD-C09E03387E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tecnológicos" sheetId="3" r:id="rId1"/>
+    <sheet name="Total" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="76">
   <si>
     <t>precio</t>
   </si>
@@ -627,13 +628,600 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CECDD3F1-1F96-4E9F-B24D-5BB0209E3DB7}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:I20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="77.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.6640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4">
+        <v>24</v>
+      </c>
+      <c r="F2" s="4">
+        <f>H2/E2</f>
+        <v>4.125</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4">
+        <v>99</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4">
+        <v>24</v>
+      </c>
+      <c r="F3" s="4">
+        <f t="shared" ref="F3:F20" si="0">H3/E3</f>
+        <v>4.125</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4">
+        <v>99</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="4">
+        <v>24</v>
+      </c>
+      <c r="F4" s="4">
+        <f t="shared" si="0"/>
+        <v>4.125</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4">
+        <v>99</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="4">
+        <v>24</v>
+      </c>
+      <c r="F5" s="4">
+        <f t="shared" si="0"/>
+        <v>4.125</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4">
+        <v>99</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4">
+        <v>16</v>
+      </c>
+      <c r="F6" s="4">
+        <f t="shared" si="0"/>
+        <v>5.625</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4">
+        <v>90</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="4">
+        <v>32</v>
+      </c>
+      <c r="F7" s="4">
+        <f t="shared" si="0"/>
+        <v>3.75</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4">
+        <v>120</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="4">
+        <v>32</v>
+      </c>
+      <c r="F8" s="4">
+        <f t="shared" si="0"/>
+        <v>3.75</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4">
+        <v>120</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="4">
+        <v>24</v>
+      </c>
+      <c r="F9" s="4">
+        <f t="shared" si="0"/>
+        <v>4.125</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4">
+        <v>99</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="4">
+        <v>48</v>
+      </c>
+      <c r="F10" s="4">
+        <f t="shared" si="0"/>
+        <v>2.9166666666666665</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4">
+        <v>140</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="4">
+        <v>48</v>
+      </c>
+      <c r="F11" s="4">
+        <f t="shared" si="0"/>
+        <v>2.9166666666666665</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4">
+        <v>140</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="4">
+        <v>24</v>
+      </c>
+      <c r="F12" s="4">
+        <f t="shared" si="0"/>
+        <v>3.2916666666666665</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4">
+        <v>79</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="4">
+        <v>24</v>
+      </c>
+      <c r="F13" s="4">
+        <f t="shared" si="0"/>
+        <v>3.2916666666666665</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4">
+        <v>79</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="4">
+        <v>24</v>
+      </c>
+      <c r="F14" s="4">
+        <f t="shared" si="0"/>
+        <v>3.2916666666666665</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4">
+        <v>79</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="4">
+        <v>24</v>
+      </c>
+      <c r="F15" s="4">
+        <f t="shared" si="0"/>
+        <v>3.2916666666666665</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4">
+        <v>79</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="4">
+        <v>24</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" si="0"/>
+        <v>3.2916666666666665</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4">
+        <v>79</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="4">
+        <v>24</v>
+      </c>
+      <c r="F17" s="4">
+        <f t="shared" si="0"/>
+        <v>3.2916666666666665</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4">
+        <v>79</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="4">
+        <v>120</v>
+      </c>
+      <c r="F18" s="4">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4">
+        <v>540</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="4">
+        <v>32</v>
+      </c>
+      <c r="F19" s="4">
+        <f t="shared" si="0"/>
+        <v>18.75</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4">
+        <v>600</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="1" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="4">
+        <v>40</v>
+      </c>
+      <c r="F20" s="4">
+        <f t="shared" si="0"/>
+        <v>4.2249999999999996</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4">
+        <v>169</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>

</xml_diff>